<commit_message>
add check menu&footer link function
</commit_message>
<xml_diff>
--- a/proj04_touringdemo/data/MY19_FXDR_Market_Matrix.xlsx
+++ b/proj04_touringdemo/data/MY19_FXDR_Market_Matrix.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\mollen\HD\AutoProject\HDAllAutoSiteV2\proj04_touringdemo\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\mollen\HD\AutoProject\HDAllAutoSitesV3\proj04_touringdemo\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="176">
   <si>
     <t>Region</t>
   </si>
@@ -570,6 +570,15 @@
   </si>
   <si>
     <t>https://ridefree.harley-davidson.com/ru_RU/thankyou</t>
+  </si>
+  <si>
+    <t>en_AU</t>
+  </si>
+  <si>
+    <t>https://ridefree.harley-davidson.com/en_AU/home</t>
+  </si>
+  <si>
+    <t>https://freedom.harley-davidson.com/en_AU-Book-A-Test-Ride-Touring/</t>
   </si>
 </sst>
 </file>
@@ -968,10 +977,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:Q33"/>
+  <dimension ref="A1:Q34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3:O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1094,125 +1103,123 @@
       </c>
       <c r="Q2" s="4"/>
     </row>
-    <row r="3" spans="1:17" ht="62" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>30</v>
+        <v>173</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>70</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="D3" s="2"/>
       <c r="E3" s="3" t="s">
-        <v>74</v>
+        <v>174</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>76</v>
+        <v>175</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>12</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="P3" s="2"/>
       <c r="Q3" s="4"/>
     </row>
-    <row r="4" spans="1:17" ht="58" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" ht="62" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q4" s="4"/>
+    </row>
+    <row r="5" spans="1:17" ht="58" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="3" t="s">
+      <c r="D5" s="4"/>
+      <c r="E5" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F5" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G5" s="3" t="s">
         <v>79</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="4"/>
-    </row>
-    <row r="5" spans="1:17" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>83</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>10</v>
@@ -1246,7 +1253,7 @@
         <v>15</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>18</v>
@@ -1255,13 +1262,13 @@
         <v>80</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>10</v>
@@ -1295,22 +1302,22 @@
         <v>15</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>80</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>10</v>
@@ -1328,10 +1335,10 @@
         <v>10</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="O7" s="2" t="s">
         <v>10</v>
@@ -1339,25 +1346,27 @@
       <c r="P7" s="4"/>
       <c r="Q7" s="4"/>
     </row>
-    <row r="8" spans="1:17" ht="58" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="4"/>
+      <c r="D8" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="E8" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>10</v>
@@ -1375,10 +1384,10 @@
         <v>10</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="O8" s="2" t="s">
         <v>10</v>
@@ -1386,27 +1395,25 @@
       <c r="P8" s="4"/>
       <c r="Q8" s="4"/>
     </row>
-    <row r="9" spans="1:17" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" ht="58" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>80</v>
-      </c>
+      <c r="D9" s="4"/>
       <c r="E9" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>10</v>
@@ -1424,10 +1431,10 @@
         <v>10</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="O9" s="2" t="s">
         <v>10</v>
@@ -1440,22 +1447,22 @@
         <v>15</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>80</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>10</v>
@@ -1473,10 +1480,10 @@
         <v>10</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="O10" s="2" t="s">
         <v>10</v>
@@ -1489,7 +1496,7 @@
         <v>15</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>13</v>
@@ -1498,13 +1505,13 @@
         <v>80</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>10</v>
@@ -1522,10 +1529,10 @@
         <v>10</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="O11" s="2" t="s">
         <v>10</v>
@@ -1538,7 +1545,7 @@
         <v>15</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>13</v>
@@ -1547,13 +1554,13 @@
         <v>80</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>10</v>
@@ -1571,10 +1578,10 @@
         <v>10</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="O12" s="2" t="s">
         <v>10</v>
@@ -1587,22 +1594,22 @@
         <v>15</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>80</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>10</v>
@@ -1636,7 +1643,7 @@
         <v>15</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>22</v>
@@ -1645,13 +1652,13 @@
         <v>80</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>10</v>
@@ -1680,25 +1687,27 @@
       <c r="P14" s="4"/>
       <c r="Q14" s="4"/>
     </row>
-    <row r="15" spans="1:17" ht="58" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="4"/>
+        <v>22</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="E15" s="3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>10</v>
@@ -1732,22 +1741,20 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>80</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="D16" s="4"/>
       <c r="E16" s="3" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>10</v>
@@ -1765,10 +1772,10 @@
         <v>10</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="O16" s="2" t="s">
         <v>10</v>
@@ -1781,22 +1788,22 @@
         <v>15</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>80</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>10</v>
@@ -1830,22 +1837,22 @@
         <v>15</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>80</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>10</v>
@@ -1879,22 +1886,22 @@
         <v>15</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>80</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>10</v>
@@ -1923,27 +1930,27 @@
       <c r="P19" s="4"/>
       <c r="Q19" s="4"/>
     </row>
-    <row r="20" spans="1:17" ht="124.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:17" ht="58" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>80</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>10</v>
@@ -1961,17 +1968,15 @@
         <v>10</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="O20" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="P20" s="2" t="s">
-        <v>129</v>
-      </c>
+      <c r="P20" s="4"/>
       <c r="Q20" s="4"/>
     </row>
     <row r="21" spans="1:17" ht="124.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1979,22 +1984,22 @@
         <v>15</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>80</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>10</v>
@@ -2025,27 +2030,27 @@
       </c>
       <c r="Q21" s="4"/>
     </row>
-    <row r="22" spans="1:17" ht="72" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:17" ht="124.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>80</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>10</v>
@@ -2076,48 +2081,48 @@
       </c>
       <c r="Q22" s="4"/>
     </row>
-    <row r="23" spans="1:17" ht="124.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:17" ht="72" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>80</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="H23" s="5" t="s">
-        <v>139</v>
+        <v>135</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="I23" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J23" s="5" t="s">
-        <v>139</v>
+      <c r="J23" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="K23" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L23" s="5" t="s">
-        <v>139</v>
+      <c r="L23" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N23" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="O23" s="2" t="s">
         <v>10</v>
@@ -2127,27 +2132,27 @@
       </c>
       <c r="Q23" s="4"/>
     </row>
-    <row r="24" spans="1:17" ht="68.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:17" ht="124.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>80</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="H24" s="5" t="s">
         <v>139</v>
@@ -2155,8 +2160,8 @@
       <c r="I24" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J24" s="2" t="s">
-        <v>11</v>
+      <c r="J24" s="5" t="s">
+        <v>139</v>
       </c>
       <c r="K24" s="2" t="s">
         <v>11</v>
@@ -2178,42 +2183,42 @@
       </c>
       <c r="Q24" s="4"/>
     </row>
-    <row r="25" spans="1:17" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:17" ht="68.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>80</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>10</v>
+        <v>142</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>139</v>
       </c>
       <c r="I25" s="2" t="s">
         <v>10</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="K25" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L25" s="2" t="s">
-        <v>10</v>
+      <c r="L25" s="5" t="s">
+        <v>139</v>
       </c>
       <c r="M25" s="2" t="s">
         <v>11</v>
@@ -2224,7 +2229,9 @@
       <c r="O25" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="P25" s="4"/>
+      <c r="P25" s="2" t="s">
+        <v>129</v>
+      </c>
       <c r="Q25" s="4"/>
     </row>
     <row r="26" spans="1:17" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2232,22 +2239,22 @@
         <v>15</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>80</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>10</v>
@@ -2281,22 +2288,22 @@
         <v>15</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>80</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>10</v>
@@ -2330,22 +2337,22 @@
         <v>15</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>80</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>10</v>
@@ -2379,22 +2386,22 @@
         <v>15</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>80</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>10</v>
@@ -2423,30 +2430,30 @@
       <c r="P29" s="4"/>
       <c r="Q29" s="4"/>
     </row>
-    <row r="30" spans="1:17" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:17" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>158</v>
+        <v>80</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I30" s="2" t="s">
         <v>10</v>
@@ -2467,44 +2474,44 @@
         <v>11</v>
       </c>
       <c r="O30" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="P30" s="4"/>
-      <c r="Q30" s="2" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" ht="62" x14ac:dyDescent="0.35">
+      <c r="Q30" s="4"/>
+    </row>
+    <row r="31" spans="1:17" ht="50" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="G31" s="4"/>
+        <v>160</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>161</v>
+      </c>
       <c r="H31" s="2" t="s">
         <v>11</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="L31" s="2" t="s">
         <v>10</v>
@@ -2516,83 +2523,83 @@
         <v>11</v>
       </c>
       <c r="O31" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="P31" s="4"/>
       <c r="Q31" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" ht="62" x14ac:dyDescent="0.35">
+      <c r="A32" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="G32" s="4"/>
+      <c r="H32" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K32" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L32" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M32" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N32" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O32" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="P32" s="4"/>
+      <c r="Q32" s="2" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="32" spans="1:17" ht="58" x14ac:dyDescent="0.35">
-      <c r="A32" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="G32" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I32" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J32" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="K32" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L32" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M32" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="N32" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="O32" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="P32" s="4"/>
-      <c r="Q32" s="4"/>
     </row>
     <row r="33" spans="1:17" ht="58" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>80</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H33" s="2" t="s">
         <v>10</v>
@@ -2604,123 +2611,174 @@
         <v>10</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L33" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M33" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="N33" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="O33" s="2" t="s">
         <v>10</v>
       </c>
       <c r="P33" s="4"/>
       <c r="Q33" s="4"/>
+    </row>
+    <row r="34" spans="1:17" ht="58" x14ac:dyDescent="0.35">
+      <c r="A34" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L34" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M34" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N34" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="O34" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="P34" s="4"/>
+      <c r="Q34" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1"/>
     <hyperlink ref="F2" r:id="rId2"/>
     <hyperlink ref="G2" r:id="rId3"/>
-    <hyperlink ref="E3" r:id="rId4"/>
-    <hyperlink ref="F3" r:id="rId5"/>
-    <hyperlink ref="G3" r:id="rId6"/>
-    <hyperlink ref="E4" r:id="rId7"/>
-    <hyperlink ref="F4" r:id="rId8"/>
-    <hyperlink ref="G4" r:id="rId9"/>
-    <hyperlink ref="E5" r:id="rId10"/>
-    <hyperlink ref="F5" r:id="rId11"/>
-    <hyperlink ref="G5" r:id="rId12"/>
-    <hyperlink ref="E6" r:id="rId13"/>
-    <hyperlink ref="F6" r:id="rId14"/>
-    <hyperlink ref="G6" r:id="rId15"/>
-    <hyperlink ref="E7" r:id="rId16"/>
-    <hyperlink ref="F7" r:id="rId17"/>
-    <hyperlink ref="G7" r:id="rId18"/>
-    <hyperlink ref="E8" r:id="rId19"/>
-    <hyperlink ref="F8" r:id="rId20"/>
-    <hyperlink ref="G8" r:id="rId21"/>
-    <hyperlink ref="E9" r:id="rId22"/>
-    <hyperlink ref="F9" r:id="rId23"/>
-    <hyperlink ref="G9" r:id="rId24"/>
-    <hyperlink ref="E10" r:id="rId25"/>
-    <hyperlink ref="F10" r:id="rId26"/>
-    <hyperlink ref="G10" r:id="rId27"/>
-    <hyperlink ref="E11" r:id="rId28"/>
-    <hyperlink ref="F11" r:id="rId29"/>
-    <hyperlink ref="G11" r:id="rId30"/>
-    <hyperlink ref="E12" r:id="rId31"/>
-    <hyperlink ref="F12" r:id="rId32"/>
-    <hyperlink ref="G12" r:id="rId33"/>
-    <hyperlink ref="E13" r:id="rId34"/>
-    <hyperlink ref="F13" r:id="rId35"/>
-    <hyperlink ref="G13" r:id="rId36"/>
-    <hyperlink ref="E14" r:id="rId37"/>
-    <hyperlink ref="F14" r:id="rId38"/>
-    <hyperlink ref="G14" r:id="rId39"/>
-    <hyperlink ref="E15" r:id="rId40"/>
-    <hyperlink ref="F15" r:id="rId41"/>
-    <hyperlink ref="G15" r:id="rId42"/>
-    <hyperlink ref="E16" r:id="rId43"/>
-    <hyperlink ref="F16" r:id="rId44"/>
-    <hyperlink ref="G16" r:id="rId45"/>
-    <hyperlink ref="E17" r:id="rId46"/>
-    <hyperlink ref="F17" r:id="rId47"/>
-    <hyperlink ref="G17" r:id="rId48"/>
-    <hyperlink ref="E18" r:id="rId49"/>
-    <hyperlink ref="F18" r:id="rId50"/>
-    <hyperlink ref="G18" r:id="rId51"/>
-    <hyperlink ref="E19" r:id="rId52"/>
-    <hyperlink ref="F19" r:id="rId53"/>
-    <hyperlink ref="G19" r:id="rId54"/>
-    <hyperlink ref="E20" r:id="rId55"/>
-    <hyperlink ref="F20" r:id="rId56"/>
-    <hyperlink ref="G20" r:id="rId57"/>
-    <hyperlink ref="E21" r:id="rId58"/>
-    <hyperlink ref="F21" r:id="rId59"/>
-    <hyperlink ref="G21" r:id="rId60"/>
-    <hyperlink ref="E22" r:id="rId61"/>
-    <hyperlink ref="F22" r:id="rId62"/>
-    <hyperlink ref="G22" r:id="rId63"/>
-    <hyperlink ref="E23" r:id="rId64"/>
-    <hyperlink ref="F23" r:id="rId65"/>
-    <hyperlink ref="G23" r:id="rId66"/>
-    <hyperlink ref="E24" r:id="rId67"/>
-    <hyperlink ref="F24" r:id="rId68"/>
-    <hyperlink ref="G24" r:id="rId69"/>
-    <hyperlink ref="E25" r:id="rId70"/>
-    <hyperlink ref="F25" r:id="rId71"/>
-    <hyperlink ref="G25" r:id="rId72"/>
-    <hyperlink ref="E26" r:id="rId73"/>
-    <hyperlink ref="F26" r:id="rId74"/>
-    <hyperlink ref="G26" r:id="rId75"/>
-    <hyperlink ref="E27" r:id="rId76"/>
-    <hyperlink ref="F27" r:id="rId77"/>
-    <hyperlink ref="G27" r:id="rId78"/>
-    <hyperlink ref="E28" r:id="rId79"/>
-    <hyperlink ref="F28" r:id="rId80"/>
-    <hyperlink ref="G28" r:id="rId81"/>
-    <hyperlink ref="E29" r:id="rId82"/>
-    <hyperlink ref="F29" r:id="rId83"/>
-    <hyperlink ref="G29" r:id="rId84"/>
-    <hyperlink ref="E30" r:id="rId85"/>
-    <hyperlink ref="F30" r:id="rId86"/>
-    <hyperlink ref="G30" r:id="rId87"/>
-    <hyperlink ref="E31" r:id="rId88"/>
-    <hyperlink ref="F31" r:id="rId89"/>
-    <hyperlink ref="E32" r:id="rId90"/>
-    <hyperlink ref="F32" r:id="rId91"/>
-    <hyperlink ref="G32" r:id="rId92"/>
-    <hyperlink ref="E33" r:id="rId93"/>
-    <hyperlink ref="F33" r:id="rId94"/>
-    <hyperlink ref="G33" r:id="rId95"/>
+    <hyperlink ref="E4" r:id="rId4"/>
+    <hyperlink ref="F4" r:id="rId5"/>
+    <hyperlink ref="G4" r:id="rId6"/>
+    <hyperlink ref="E5" r:id="rId7"/>
+    <hyperlink ref="F5" r:id="rId8"/>
+    <hyperlink ref="G5" r:id="rId9"/>
+    <hyperlink ref="E6" r:id="rId10"/>
+    <hyperlink ref="F6" r:id="rId11"/>
+    <hyperlink ref="G6" r:id="rId12"/>
+    <hyperlink ref="E7" r:id="rId13"/>
+    <hyperlink ref="F7" r:id="rId14"/>
+    <hyperlink ref="G7" r:id="rId15"/>
+    <hyperlink ref="E8" r:id="rId16"/>
+    <hyperlink ref="F8" r:id="rId17"/>
+    <hyperlink ref="G8" r:id="rId18"/>
+    <hyperlink ref="E9" r:id="rId19"/>
+    <hyperlink ref="F9" r:id="rId20"/>
+    <hyperlink ref="G9" r:id="rId21"/>
+    <hyperlink ref="E10" r:id="rId22"/>
+    <hyperlink ref="F10" r:id="rId23"/>
+    <hyperlink ref="G10" r:id="rId24"/>
+    <hyperlink ref="E11" r:id="rId25"/>
+    <hyperlink ref="F11" r:id="rId26"/>
+    <hyperlink ref="G11" r:id="rId27"/>
+    <hyperlink ref="E12" r:id="rId28"/>
+    <hyperlink ref="F12" r:id="rId29"/>
+    <hyperlink ref="G12" r:id="rId30"/>
+    <hyperlink ref="E13" r:id="rId31"/>
+    <hyperlink ref="F13" r:id="rId32"/>
+    <hyperlink ref="G13" r:id="rId33"/>
+    <hyperlink ref="E14" r:id="rId34"/>
+    <hyperlink ref="F14" r:id="rId35"/>
+    <hyperlink ref="G14" r:id="rId36"/>
+    <hyperlink ref="E15" r:id="rId37"/>
+    <hyperlink ref="F15" r:id="rId38"/>
+    <hyperlink ref="G15" r:id="rId39"/>
+    <hyperlink ref="E16" r:id="rId40"/>
+    <hyperlink ref="F16" r:id="rId41"/>
+    <hyperlink ref="G16" r:id="rId42"/>
+    <hyperlink ref="E17" r:id="rId43"/>
+    <hyperlink ref="F17" r:id="rId44"/>
+    <hyperlink ref="G17" r:id="rId45"/>
+    <hyperlink ref="E18" r:id="rId46"/>
+    <hyperlink ref="F18" r:id="rId47"/>
+    <hyperlink ref="G18" r:id="rId48"/>
+    <hyperlink ref="E19" r:id="rId49"/>
+    <hyperlink ref="F19" r:id="rId50"/>
+    <hyperlink ref="G19" r:id="rId51"/>
+    <hyperlink ref="E20" r:id="rId52"/>
+    <hyperlink ref="F20" r:id="rId53"/>
+    <hyperlink ref="G20" r:id="rId54"/>
+    <hyperlink ref="E21" r:id="rId55"/>
+    <hyperlink ref="F21" r:id="rId56"/>
+    <hyperlink ref="G21" r:id="rId57"/>
+    <hyperlink ref="E22" r:id="rId58"/>
+    <hyperlink ref="F22" r:id="rId59"/>
+    <hyperlink ref="G22" r:id="rId60"/>
+    <hyperlink ref="E23" r:id="rId61"/>
+    <hyperlink ref="F23" r:id="rId62"/>
+    <hyperlink ref="G23" r:id="rId63"/>
+    <hyperlink ref="E24" r:id="rId64"/>
+    <hyperlink ref="F24" r:id="rId65"/>
+    <hyperlink ref="G24" r:id="rId66"/>
+    <hyperlink ref="E25" r:id="rId67"/>
+    <hyperlink ref="F25" r:id="rId68"/>
+    <hyperlink ref="G25" r:id="rId69"/>
+    <hyperlink ref="E26" r:id="rId70"/>
+    <hyperlink ref="F26" r:id="rId71"/>
+    <hyperlink ref="G26" r:id="rId72"/>
+    <hyperlink ref="E27" r:id="rId73"/>
+    <hyperlink ref="F27" r:id="rId74"/>
+    <hyperlink ref="G27" r:id="rId75"/>
+    <hyperlink ref="E28" r:id="rId76"/>
+    <hyperlink ref="F28" r:id="rId77"/>
+    <hyperlink ref="G28" r:id="rId78"/>
+    <hyperlink ref="E29" r:id="rId79"/>
+    <hyperlink ref="F29" r:id="rId80"/>
+    <hyperlink ref="G29" r:id="rId81"/>
+    <hyperlink ref="E30" r:id="rId82"/>
+    <hyperlink ref="F30" r:id="rId83"/>
+    <hyperlink ref="G30" r:id="rId84"/>
+    <hyperlink ref="E31" r:id="rId85"/>
+    <hyperlink ref="F31" r:id="rId86"/>
+    <hyperlink ref="G31" r:id="rId87"/>
+    <hyperlink ref="E32" r:id="rId88"/>
+    <hyperlink ref="F32" r:id="rId89"/>
+    <hyperlink ref="E33" r:id="rId90"/>
+    <hyperlink ref="F33" r:id="rId91"/>
+    <hyperlink ref="G33" r:id="rId92"/>
+    <hyperlink ref="E34" r:id="rId93"/>
+    <hyperlink ref="F34" r:id="rId94"/>
+    <hyperlink ref="G34" r:id="rId95"/>
+    <hyperlink ref="E3" r:id="rId96"/>
+    <hyperlink ref="F3" r:id="rId97"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId96"/>
+  <pageSetup orientation="portrait" r:id="rId98"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
update header&menu error code
</commit_message>
<xml_diff>
--- a/proj04_touringdemo/data/MY19_FXDR_Market_Matrix.xlsx
+++ b/proj04_touringdemo/data/MY19_FXDR_Market_Matrix.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="171">
   <si>
     <t>Region</t>
   </si>
@@ -106,9 +106,6 @@
     <t>Swedish</t>
   </si>
   <si>
-    <t>Turkish</t>
-  </si>
-  <si>
     <t>en_CA</t>
   </si>
   <si>
@@ -130,9 +127,6 @@
     <t>es_MX</t>
   </si>
   <si>
-    <t>tr_TR</t>
-  </si>
-  <si>
     <t>sv_SE</t>
   </si>
   <si>
@@ -178,9 +172,6 @@
     <t>en_ZZ</t>
   </si>
   <si>
-    <t>el_GR</t>
-  </si>
-  <si>
     <t>en_IE</t>
   </si>
   <si>
@@ -292,15 +283,6 @@
     <t>https://ridefree.harley-davidson.com/en_GB/thankyou</t>
   </si>
   <si>
-    <t>https://ridefree.harley-davidson.com/el_GR/home</t>
-  </si>
-  <si>
-    <t>https://ridefree.harley-davidson.com/el_GR/booking</t>
-  </si>
-  <si>
-    <t>https://ridefree.harley-davidson.com/el_GR/thankyou</t>
-  </si>
-  <si>
     <t>https://ridefree.harley-davidson.com/en_IE/home</t>
   </si>
   <si>
@@ -353,15 +335,6 @@
   </si>
   <si>
     <t>https://ridefree.harley-davidson.com/nl_NL/thankyou</t>
-  </si>
-  <si>
-    <t>https://ridefree.harley-davidson.com/tr_TR/home</t>
-  </si>
-  <si>
-    <t>https://ridefree.harley-davidson.com/tr_TR/booking</t>
-  </si>
-  <si>
-    <t>https://ridefree.harley-davidson.com/tr_TR/thankyou</t>
   </si>
   <si>
     <t>https://ridefree.harley-davidson.com/cs_CZ/home</t>
@@ -579,6 +552,18 @@
   </si>
   <si>
     <t>https://freedom.harley-davidson.com/en_AU-Book-A-Test-Ride-Touring/</t>
+  </si>
+  <si>
+    <t>Open road freedom starts here. Take a test ride for the chance to win a dream adventure on a new 2019 #Harley Touring bike.</t>
+  </si>
+  <si>
+    <t>TranslationValue</t>
+  </si>
+  <si>
+    <t>La liberté commence ici.  Réalisez un essai pour avoir une chance de gagner un voyage de rêve sur un nouveau modèle #Touring 2019 Harley.</t>
+  </si>
+  <si>
+    <t>Die Freiheit der Straße beginnt hier.  Machen Sie eine Probefahrt und wahren Sie die Chance, ein Traumabenteuer auf einem neuen 2019er #Harley Touring Bike zu gewinnen.</t>
   </si>
 </sst>
 </file>
@@ -977,10 +962,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:Q34"/>
+  <dimension ref="A1:R32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3:O3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -996,10 +981,10 @@
     <col min="9" max="9" width="18.453125" customWidth="1"/>
     <col min="10" max="13" width="19.54296875" customWidth="1"/>
     <col min="14" max="14" width="18.453125" customWidth="1"/>
-    <col min="15" max="15" width="37.6328125" customWidth="1"/>
+    <col min="15" max="16" width="37.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" ht="30" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1010,7 +995,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -1022,58 +1007,61 @@
         <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="P1" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="Q1" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="62" x14ac:dyDescent="0.35">
+      <c r="R1" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="62" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>73</v>
-      </c>
       <c r="H2" s="2" t="s">
         <v>10</v>
       </c>
@@ -1099,26 +1087,29 @@
         <v>10</v>
       </c>
       <c r="P2" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="Q2" s="4"/>
-    </row>
-    <row r="3" spans="1:17" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="R2" s="4"/>
+    </row>
+    <row r="3" spans="1:18" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="3" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>11</v>
@@ -1147,30 +1138,33 @@
       <c r="O3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="4"/>
-    </row>
-    <row r="4" spans="1:17" ht="62" x14ac:dyDescent="0.35">
+      <c r="P3" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="4"/>
+    </row>
+    <row r="4" spans="1:18" ht="62" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>10</v>
@@ -1197,29 +1191,32 @@
         <v>10</v>
       </c>
       <c r="P4" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="Q4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="Q4" s="4"/>
-    </row>
-    <row r="5" spans="1:17" ht="58" x14ac:dyDescent="0.35">
+      <c r="R4" s="4"/>
+    </row>
+    <row r="5" spans="1:18" ht="58" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>10</v>
@@ -1245,31 +1242,32 @@
       <c r="O5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="P5" s="4"/>
+      <c r="P5" s="2"/>
       <c r="Q5" s="4"/>
-    </row>
-    <row r="6" spans="1:17" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="R5" s="4"/>
+    </row>
+    <row r="6" spans="1:18" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>83</v>
-      </c>
       <c r="H6" s="2" t="s">
         <v>10</v>
       </c>
@@ -1294,30 +1292,33 @@
       <c r="O6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="P6" s="4"/>
+      <c r="P6" s="2" t="s">
+        <v>170</v>
+      </c>
       <c r="Q6" s="4"/>
-    </row>
-    <row r="7" spans="1:17" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="R6" s="4"/>
+    </row>
+    <row r="7" spans="1:18" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>10</v>
@@ -1343,30 +1344,33 @@
       <c r="O7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="P7" s="4"/>
+      <c r="P7" s="2" t="s">
+        <v>170</v>
+      </c>
       <c r="Q7" s="4"/>
-    </row>
-    <row r="8" spans="1:17" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="R7" s="4"/>
+    </row>
+    <row r="8" spans="1:18" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>10</v>
@@ -1392,28 +1396,33 @@
       <c r="O8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="P8" s="4"/>
+      <c r="P8" s="2" t="s">
+        <v>167</v>
+      </c>
       <c r="Q8" s="4"/>
-    </row>
-    <row r="9" spans="1:17" ht="58" x14ac:dyDescent="0.35">
+      <c r="R8" s="4"/>
+    </row>
+    <row r="9" spans="1:18" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="4"/>
+      <c r="D9" s="2" t="s">
+        <v>77</v>
+      </c>
       <c r="E9" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>10</v>
@@ -1431,38 +1440,39 @@
         <v>10</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="O9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="P9" s="4"/>
+      <c r="P9" s="2"/>
       <c r="Q9" s="4"/>
-    </row>
-    <row r="10" spans="1:17" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="R9" s="4"/>
+    </row>
+    <row r="10" spans="1:18" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>10</v>
@@ -1480,38 +1490,39 @@
         <v>10</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="O10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="P10" s="4"/>
+      <c r="P10" s="2"/>
       <c r="Q10" s="4"/>
-    </row>
-    <row r="11" spans="1:17" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="R10" s="4"/>
+    </row>
+    <row r="11" spans="1:18" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>10</v>
@@ -1529,38 +1540,39 @@
         <v>10</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="O11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="P11" s="4"/>
+      <c r="P11" s="2"/>
       <c r="Q11" s="4"/>
-    </row>
-    <row r="12" spans="1:17" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="R11" s="4"/>
+    </row>
+    <row r="12" spans="1:18" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>10</v>
@@ -1578,38 +1590,39 @@
         <v>10</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="O12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="P12" s="4"/>
+      <c r="P12" s="2"/>
       <c r="Q12" s="4"/>
-    </row>
-    <row r="13" spans="1:17" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="R12" s="4"/>
+    </row>
+    <row r="13" spans="1:18" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>10</v>
@@ -1635,30 +1648,31 @@
       <c r="O13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="P13" s="4"/>
+      <c r="P13" s="2"/>
       <c r="Q13" s="4"/>
-    </row>
-    <row r="14" spans="1:17" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="R13" s="4"/>
+    </row>
+    <row r="14" spans="1:18" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>10</v>
@@ -1684,30 +1698,31 @@
       <c r="O14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="P14" s="4"/>
+      <c r="P14" s="2"/>
       <c r="Q14" s="4"/>
-    </row>
-    <row r="15" spans="1:17" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="R14" s="4"/>
+    </row>
+    <row r="15" spans="1:18" ht="58" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>10</v>
@@ -1725,36 +1740,39 @@
         <v>10</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="O15" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="P15" s="4"/>
+      <c r="P15" s="2"/>
       <c r="Q15" s="4"/>
-    </row>
-    <row r="16" spans="1:17" ht="58" x14ac:dyDescent="0.35">
+      <c r="R15" s="4"/>
+    </row>
+    <row r="16" spans="1:18" ht="58" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>77</v>
+      </c>
       <c r="E16" s="3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>10</v>
@@ -1772,38 +1790,39 @@
         <v>10</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="O16" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="P16" s="4"/>
+      <c r="P16" s="2"/>
       <c r="Q16" s="4"/>
-    </row>
-    <row r="17" spans="1:17" ht="58" x14ac:dyDescent="0.35">
+      <c r="R16" s="4"/>
+    </row>
+    <row r="17" spans="1:18" ht="58" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>10</v>
@@ -1829,30 +1848,31 @@
       <c r="O17" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="P17" s="4"/>
+      <c r="P17" s="2"/>
       <c r="Q17" s="4"/>
-    </row>
-    <row r="18" spans="1:17" ht="58" x14ac:dyDescent="0.35">
+      <c r="R17" s="4"/>
+    </row>
+    <row r="18" spans="1:18" ht="58" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>10</v>
@@ -1878,80 +1898,84 @@
       <c r="O18" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="P18" s="4"/>
+      <c r="P18" s="2"/>
       <c r="Q18" s="4"/>
-    </row>
-    <row r="19" spans="1:17" ht="58" x14ac:dyDescent="0.35">
+      <c r="R18" s="4"/>
+    </row>
+    <row r="19" spans="1:18" ht="124.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E19" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="O19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="F19" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="K19" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L19" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="M19" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="N19" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="O19" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="P19" s="4"/>
-      <c r="Q19" s="4"/>
-    </row>
-    <row r="20" spans="1:17" ht="58" x14ac:dyDescent="0.35">
+      <c r="R19" s="4"/>
+    </row>
+    <row r="20" spans="1:18" ht="124.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E20" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="G20" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="F20" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>125</v>
-      </c>
       <c r="H20" s="2" t="s">
         <v>10</v>
       </c>
@@ -1968,39 +1992,42 @@
         <v>10</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="O20" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="P20" s="4"/>
-      <c r="Q20" s="4"/>
-    </row>
-    <row r="21" spans="1:17" ht="124.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P20" s="2"/>
+      <c r="Q20" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="R20" s="4"/>
+    </row>
+    <row r="21" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E21" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="G21" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="F21" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>128</v>
-      </c>
       <c r="H21" s="2" t="s">
         <v>10</v>
       </c>
@@ -2025,149 +2052,152 @@
       <c r="O21" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="P21" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="Q21" s="4"/>
-    </row>
-    <row r="22" spans="1:17" ht="124.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P21" s="2"/>
+      <c r="Q21" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="R21" s="4"/>
+    </row>
+    <row r="22" spans="1:18" ht="124.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E22" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="H22" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="F22" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="I22" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J22" s="2" t="s">
-        <v>10</v>
+      <c r="J22" s="5" t="s">
+        <v>130</v>
       </c>
       <c r="K22" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L22" s="2" t="s">
-        <v>10</v>
+      <c r="L22" s="5" t="s">
+        <v>130</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="O22" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="P22" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="Q22" s="4"/>
-    </row>
-    <row r="23" spans="1:17" ht="72" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P22" s="2"/>
+      <c r="Q22" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="R22" s="4"/>
+    </row>
+    <row r="23" spans="1:18" ht="68.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E23" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="G23" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="F23" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>10</v>
+      <c r="H23" s="5" t="s">
+        <v>130</v>
       </c>
       <c r="I23" s="2" t="s">
         <v>10</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="K23" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L23" s="2" t="s">
-        <v>10</v>
+      <c r="L23" s="5" t="s">
+        <v>130</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="N23" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="O23" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="P23" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="Q23" s="4"/>
-    </row>
-    <row r="24" spans="1:17" ht="124.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="R23" s="4"/>
+    </row>
+    <row r="24" spans="1:18" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E24" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="G24" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="F24" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="H24" s="5" t="s">
-        <v>139</v>
+      <c r="H24" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="I24" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J24" s="5" t="s">
-        <v>139</v>
+      <c r="J24" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="K24" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L24" s="5" t="s">
-        <v>139</v>
+      <c r="L24" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="M24" s="2" t="s">
         <v>11</v>
@@ -2178,12 +2208,11 @@
       <c r="O24" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="P24" s="2" t="s">
-        <v>129</v>
-      </c>
+      <c r="P24" s="2"/>
       <c r="Q24" s="4"/>
-    </row>
-    <row r="25" spans="1:17" ht="68.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="R24" s="4"/>
+    </row>
+    <row r="25" spans="1:18" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>15</v>
       </c>
@@ -2191,34 +2220,34 @@
         <v>39</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="H25" s="5" t="s">
         <v>139</v>
       </c>
+      <c r="H25" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="I25" s="2" t="s">
         <v>10</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K25" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L25" s="5" t="s">
-        <v>139</v>
+      <c r="L25" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="M25" s="2" t="s">
         <v>11</v>
@@ -2229,32 +2258,31 @@
       <c r="O25" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="P25" s="2" t="s">
-        <v>129</v>
-      </c>
+      <c r="P25" s="2"/>
       <c r="Q25" s="4"/>
-    </row>
-    <row r="26" spans="1:17" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="R25" s="4"/>
+    </row>
+    <row r="26" spans="1:18" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>10</v>
@@ -2280,30 +2308,31 @@
       <c r="O26" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="P26" s="4"/>
+      <c r="P26" s="2"/>
       <c r="Q26" s="4"/>
-    </row>
-    <row r="27" spans="1:17" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="R26" s="4"/>
+    </row>
+    <row r="27" spans="1:18" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>10</v>
@@ -2329,119 +2358,124 @@
       <c r="O27" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="P27" s="4"/>
+      <c r="P27" s="2"/>
       <c r="Q27" s="4"/>
-    </row>
-    <row r="28" spans="1:17" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="R27" s="4"/>
+    </row>
+    <row r="28" spans="1:18" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E28" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L28" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M28" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N28" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O28" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="P28" s="2"/>
+      <c r="Q28" s="4"/>
+      <c r="R28" s="4"/>
+    </row>
+    <row r="29" spans="1:18" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="F28" s="3" t="s">
+      <c r="E29" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="G28" s="3" t="s">
+      <c r="F29" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="H28" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I28" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J28" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="K28" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L28" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="M28" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="N28" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="O28" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="P28" s="4"/>
-      <c r="Q28" s="4"/>
-    </row>
-    <row r="29" spans="1:17" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B29" s="2" t="s">
+      <c r="G29" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L29" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M29" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N29" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O29" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="P29" s="2"/>
+      <c r="Q29" s="4"/>
+      <c r="R29" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" ht="62" x14ac:dyDescent="0.35">
+      <c r="A30" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="G29" s="3" t="s">
+      <c r="C30" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>154</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I29" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J29" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="K29" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L29" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="M29" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="N29" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="O29" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="P29" s="4"/>
-      <c r="Q29" s="4"/>
-    </row>
-    <row r="30" spans="1:17" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>80</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>155</v>
@@ -2449,233 +2483,136 @@
       <c r="F30" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="G30" s="3" t="s">
+      <c r="G30" s="4"/>
+      <c r="H30" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L30" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M30" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N30" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O30" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="P30" s="2"/>
+      <c r="Q30" s="4"/>
+      <c r="R30" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="H30" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I30" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J30" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="K30" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L30" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="M30" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="N30" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="O30" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="P30" s="4"/>
-      <c r="Q30" s="4"/>
-    </row>
-    <row r="31" spans="1:17" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="31" spans="1:18" ht="58" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D31" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E31" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="F31" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="F31" s="3" t="s">
+      <c r="G31" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="G31" s="3" t="s">
+      <c r="H31" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L31" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M31" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N31" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O31" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="P31" s="2"/>
+      <c r="Q31" s="4"/>
+      <c r="R31" s="4"/>
+    </row>
+    <row r="32" spans="1:18" ht="58" x14ac:dyDescent="0.35">
+      <c r="A32" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E32" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="H31" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I31" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J31" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="K31" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L31" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="M31" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="N31" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="O31" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="P31" s="4"/>
-      <c r="Q31" s="2" t="s">
+      <c r="F32" s="3" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="32" spans="1:17" ht="62" x14ac:dyDescent="0.35">
-      <c r="A32" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D32" s="2" t="s">
+      <c r="G32" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="E32" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="G32" s="4"/>
       <c r="H32" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="L32" s="2" t="s">
         <v>10</v>
       </c>
       <c r="M32" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N32" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="O32" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="P32" s="4"/>
-      <c r="Q32" s="2" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" ht="58" x14ac:dyDescent="0.35">
-      <c r="A33" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="G33" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I33" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J33" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="K33" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L33" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M33" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="N33" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="O33" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="P33" s="4"/>
-      <c r="Q33" s="4"/>
-    </row>
-    <row r="34" spans="1:17" ht="58" x14ac:dyDescent="0.35">
-      <c r="A34" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="G34" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="H34" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I34" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J34" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="K34" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L34" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="M34" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="N34" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="O34" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="P34" s="4"/>
-      <c r="Q34" s="4"/>
+      <c r="P32" s="2"/>
+      <c r="Q32" s="4"/>
+      <c r="R32" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2762,23 +2699,17 @@
     <hyperlink ref="G29" r:id="rId81"/>
     <hyperlink ref="E30" r:id="rId82"/>
     <hyperlink ref="F30" r:id="rId83"/>
-    <hyperlink ref="G30" r:id="rId84"/>
-    <hyperlink ref="E31" r:id="rId85"/>
-    <hyperlink ref="F31" r:id="rId86"/>
-    <hyperlink ref="G31" r:id="rId87"/>
-    <hyperlink ref="E32" r:id="rId88"/>
-    <hyperlink ref="F32" r:id="rId89"/>
-    <hyperlink ref="E33" r:id="rId90"/>
-    <hyperlink ref="F33" r:id="rId91"/>
-    <hyperlink ref="G33" r:id="rId92"/>
-    <hyperlink ref="E34" r:id="rId93"/>
-    <hyperlink ref="F34" r:id="rId94"/>
-    <hyperlink ref="G34" r:id="rId95"/>
-    <hyperlink ref="E3" r:id="rId96"/>
-    <hyperlink ref="F3" r:id="rId97"/>
+    <hyperlink ref="E31" r:id="rId84"/>
+    <hyperlink ref="F31" r:id="rId85"/>
+    <hyperlink ref="G31" r:id="rId86"/>
+    <hyperlink ref="E32" r:id="rId87"/>
+    <hyperlink ref="F32" r:id="rId88"/>
+    <hyperlink ref="G32" r:id="rId89"/>
+    <hyperlink ref="E3" r:id="rId90"/>
+    <hyperlink ref="F3" r:id="rId91"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId98"/>
+  <pageSetup orientation="portrait" r:id="rId92"/>
 </worksheet>
 </file>
 

</xml_diff>